<commit_message>
Implement names, box-coloring, uptake threshold
</commit_message>
<xml_diff>
--- a/data/namelist.xlsx
+++ b/data/namelist.xlsx
@@ -674,7 +674,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -718,9 +718,7 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
-        <v>100</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1">
@@ -729,9 +727,7 @@
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
-        <v>100</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1">
@@ -772,9 +768,7 @@
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1">
-        <v>200</v>
-      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="1">
@@ -783,6 +777,9 @@
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C11" s="1">
+        <v>300</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="1">
@@ -799,9 +796,7 @@
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1">
-        <v>50</v>
-      </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="1">
@@ -842,9 +837,7 @@
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="1">
-        <v>10</v>
-      </c>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="1">
@@ -885,9 +878,7 @@
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="1">
-        <v>200</v>
-      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="1">
@@ -912,9 +903,7 @@
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="1">
-        <v>40</v>
-      </c>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="1">

</xml_diff>